<commit_message>
Updated testing with more sensible parameters, looks much better already!
</commit_message>
<xml_diff>
--- a/testing/d0b_b.xlsx
+++ b/testing/d0b_b.xlsx
@@ -2235,10 +2235,10 @@
         <v>3</v>
       </c>
       <c r="B3" s="17">
-        <v>0.24378992322565235</v>
+        <v>-1.9770267617657384</v>
       </c>
       <c r="C3" s="20">
-        <v>0.24673946811054964</v>
+        <v>-1.9497280051420887</v>
       </c>
     </row>
     <row r="4">
@@ -2246,10 +2246,10 @@
         <v>4</v>
       </c>
       <c r="B4" s="25">
-        <v>0.38497677741070035</v>
+        <v>-2.1247586523022473</v>
       </c>
       <c r="C4" s="28">
-        <v>0.39118693679252353</v>
+        <v>-2.0719191754432713</v>
       </c>
     </row>
     <row r="5">
@@ -2257,10 +2257,10 @@
         <v>5</v>
       </c>
       <c r="B5" s="33">
-        <v>0.68157504557588933</v>
+        <v>-2.2515035901787703</v>
       </c>
       <c r="C5" s="36">
-        <v>0.6916390348355721</v>
+        <v>-2.1801205335574969</v>
       </c>
     </row>
     <row r="6">
@@ -2268,10 +2268,10 @@
         <v>6</v>
       </c>
       <c r="B6" s="41">
-        <v>1.0082832030718387</v>
+        <v>-2.2194752216690619</v>
       </c>
       <c r="C6" s="44">
-        <v>1.0225675142449915</v>
+        <v>-2.1290762581173475</v>
       </c>
     </row>
     <row r="7">
@@ -2279,10 +2279,10 @@
         <v>7</v>
       </c>
       <c r="B7" s="49">
-        <v>1.2905234710239451</v>
+        <v>-2.2626980658252043</v>
       </c>
       <c r="C7" s="52">
-        <v>1.3089635051530266</v>
+        <v>-2.1559522509384146</v>
       </c>
     </row>
     <row r="8">
@@ -2295,10 +2295,10 @@
         <v>3</v>
       </c>
       <c r="B9" s="59">
-        <v>0.37203102574438207</v>
+        <v>0.35605176398309912</v>
       </c>
       <c r="C9" s="62">
-        <v>0.37255345946071305</v>
+        <v>0.35825921679285777</v>
       </c>
     </row>
     <row r="10">
@@ -2339,10 +2339,10 @@
         <v>12</v>
       </c>
       <c r="B13" s="91">
-        <v>2.3145070215393715</v>
+        <v>0.061789755953912097</v>
       </c>
       <c r="C13" s="94">
-        <v>2.3102660287237948</v>
+        <v>0.062282729873806488</v>
       </c>
     </row>
     <row r="14">
@@ -2350,10 +2350,10 @@
         <v>13</v>
       </c>
       <c r="B14" s="99">
-        <v>7.8918354254348451</v>
+        <v>1.0792832465898308</v>
       </c>
       <c r="C14" s="102">
-        <v>7.8885261582442938</v>
+        <v>1.0782819005691589</v>
       </c>
     </row>
     <row r="15">
@@ -2366,7 +2366,7 @@
         <v>3</v>
       </c>
       <c r="C16" s="109">
-        <v>0.058727177193403063</v>
+        <v>-0.147226934973433</v>
       </c>
     </row>
     <row r="17">
@@ -2374,7 +2374,7 @@
         <v>9</v>
       </c>
       <c r="C17" s="114">
-        <v>-0.0053888854647505102</v>
+        <v>-0.021307115571185753</v>
       </c>
     </row>
     <row r="18">
@@ -2382,7 +2382,7 @@
         <v>10</v>
       </c>
       <c r="C18" s="119">
-        <v>0.0066092809849606039</v>
+        <v>0.11776015566474256</v>
       </c>
     </row>
     <row r="19">
@@ -2390,7 +2390,7 @@
         <v>11</v>
       </c>
       <c r="C19" s="124">
-        <v>-2.9947112800351734</v>
+        <v>-1.5403318388201941</v>
       </c>
     </row>
     <row r="20">
@@ -2398,7 +2398,7 @@
         <v>14</v>
       </c>
       <c r="C20" s="129">
-        <v>0.67500035230654887</v>
+        <v>0.03712047798613282</v>
       </c>
     </row>
     <row r="21">
@@ -2406,10 +2406,10 @@
         <v>15</v>
       </c>
       <c r="B21" s="136">
-        <v>7904</v>
+        <v>8259</v>
       </c>
       <c r="C21" s="140">
-        <v>9671</v>
+        <v>10222</v>
       </c>
     </row>
   </sheetData>

</xml_diff>